<commit_message>
Add complete dummy payment data - 5 recipients with various payment statuses
</commit_message>
<xml_diff>
--- a/recipients_data.xlsx
+++ b/recipients_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>¥2500</t>
+          <t>2500</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>¥500</t>
+          <t>500</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -481,6 +481,126 @@
       </c>
       <c r="F2" t="n">
         <v>2001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Service fee</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3500</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Partial payment</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ahmed Khan</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4200</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4200</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Invoice #001</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Maria Garcia</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1800</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Retainer</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>2005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplify to web-based system: admin can import/export Excel, removed all sync scripts
</commit_message>
<xml_diff>
--- a/recipients_data.xlsx
+++ b/recipients_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,26 @@
           <t>Receipt No</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Recipient Email</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Payment_Status</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Amount_Paid</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -459,15 +479,11 @@
           <t>SARWAR</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C2" t="n">
+        <v>500</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -482,126 +498,206 @@
       <c r="F2" t="n">
         <v>2001</v>
       </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3500</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1500</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Service fee</t>
+          <t>Partial payment</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2002</v>
-      </c>
+        <v>2003</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
+          <t>Test Payment</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>500</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-01T15:00:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Partial payment</t>
+          <t>Test payment for verification</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2003</v>
+        <v>9999</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>sarwarofficial2006@gmail.com</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>DUE</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>¥1500</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2026-02-01T17:34:33.169Z</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ahmed Khan</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4200</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>4200</t>
-        </is>
+          <t>Maria Garcia</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Invoice #001</t>
+          <t>Retainer</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2004</v>
-      </c>
+        <v>2005</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Maria Garcia</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1800</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Ali</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1000</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-31T15:00:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Retainer</t>
+          <t>Dummy payment</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2005</v>
-      </c>
+        <v>2006</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Service fee</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>2002</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ahmed Khan</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4200</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4200</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Invoice #001</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>2004</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>